<commit_message>
Fix multiple bug in config file and program
</commit_message>
<xml_diff>
--- a/conf/excel/C_BackLine.xlsx
+++ b/conf/excel/C_BackLine.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\学习资料\综合学习资料\tencent\配置文件相关\newCA-config-final\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\长期文件\学习资料\综合学习资料\tencent\配置文件相关\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26B1D365-3BB5-4267-99F4-5523748D4E64}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D45429CA-F93E-4678-8486-35D1B4625291}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2730" yWindow="2730" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1320" yWindow="1125" windowWidth="23580" windowHeight="10035" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="C_BackLine.conf" sheetId="1" r:id="rId1"/>
@@ -441,166 +441,166 @@
     <t>体育场范围线</t>
   </si>
   <si>
-    <t>kind%=%0242</t>
-  </si>
-  <si>
-    <t>kind%=%0243</t>
-  </si>
-  <si>
-    <t>kind%=%0244</t>
-  </si>
-  <si>
-    <t>kind%=%0241</t>
-  </si>
-  <si>
-    <t>kind%=%0245</t>
-  </si>
-  <si>
-    <t>kind%=%0246</t>
-  </si>
-  <si>
-    <t>kind%=%07ff</t>
-  </si>
-  <si>
-    <t>kind%=%010bj0103</t>
-  </si>
-  <si>
-    <t>kind%=%010bj0104</t>
-  </si>
-  <si>
-    <t>kind%=%010bj0109</t>
-  </si>
-  <si>
-    <t>kind%=%010bj0106</t>
-  </si>
-  <si>
-    <t>kind%=%010bj0107</t>
-  </si>
-  <si>
-    <t>kind%=%0010</t>
-  </si>
-  <si>
-    <t>kind%=%0136</t>
-  </si>
-  <si>
-    <t>kind%=%0137</t>
-  </si>
-  <si>
-    <t>kind%=%0133</t>
-  </si>
-  <si>
-    <t>kind%=%0134</t>
-  </si>
-  <si>
-    <t>kind%=%02ff</t>
-  </si>
-  <si>
-    <t>kind%=%0121</t>
-  </si>
-  <si>
-    <t>kind%=%0123</t>
-  </si>
-  <si>
-    <t>kind%=%0122</t>
-  </si>
-  <si>
-    <t>kind%=%0125</t>
-  </si>
-  <si>
-    <t>kind%=%0143</t>
-  </si>
-  <si>
-    <t>kind%=%0145</t>
-  </si>
-  <si>
-    <t>kind%=%0146</t>
-  </si>
-  <si>
-    <t>kind%=%0147</t>
-  </si>
-  <si>
-    <t>kind%=%0148</t>
-  </si>
-  <si>
-    <t>kind%=%0141</t>
-  </si>
-  <si>
-    <t>kind%=%0142</t>
-  </si>
-  <si>
-    <t>kind%=%0144</t>
-  </si>
-  <si>
-    <t>kind%=%0149</t>
-  </si>
-  <si>
-    <t>kind%=%014a</t>
-  </si>
-  <si>
-    <t>kind%=%014b</t>
-  </si>
-  <si>
-    <t>kind%=%01ff</t>
-  </si>
-  <si>
-    <t>kind%=%04ff</t>
-  </si>
-  <si>
-    <t>kind%=%0161</t>
-  </si>
-  <si>
-    <t>kind%=%0162</t>
-  </si>
-  <si>
-    <t>kind%=%0163</t>
-  </si>
-  <si>
-    <t>kind%=%0164</t>
-  </si>
-  <si>
-    <t>kind%=%06ff</t>
-  </si>
-  <si>
-    <t>kind%=%0165</t>
-  </si>
-  <si>
-    <t>kind%=%0166</t>
-  </si>
-  <si>
-    <t>kind%=%0167</t>
-  </si>
-  <si>
-    <t>kind%=%0171</t>
-  </si>
-  <si>
-    <t>kind%=%0172</t>
-  </si>
-  <si>
-    <t>kind%=%0173</t>
-  </si>
-  <si>
-    <t>kind%=%0174</t>
-  </si>
-  <si>
-    <t>kind%=%0175</t>
-  </si>
-  <si>
-    <t>kind%=%0176</t>
-  </si>
-  <si>
-    <t>kind%=%0177</t>
-  </si>
-  <si>
-    <t>kind%=%0178</t>
-  </si>
-  <si>
-    <t>kind%=%0179</t>
-  </si>
-  <si>
-    <t>kind%=%017a</t>
-  </si>
-  <si>
-    <t>kind%=%84ff</t>
+    <t>kind%=0144</t>
+  </si>
+  <si>
+    <t>kind%=0242</t>
+  </si>
+  <si>
+    <t>kind%=0243</t>
+  </si>
+  <si>
+    <t>kind%=0244</t>
+  </si>
+  <si>
+    <t>kind%=0241</t>
+  </si>
+  <si>
+    <t>kind%=0245</t>
+  </si>
+  <si>
+    <t>kind%=0246</t>
+  </si>
+  <si>
+    <t>kind%=07ff</t>
+  </si>
+  <si>
+    <t>kind%=010bj0103</t>
+  </si>
+  <si>
+    <t>kind%=010bj0104</t>
+  </si>
+  <si>
+    <t>kind%=010bj0109</t>
+  </si>
+  <si>
+    <t>kind%=010bj0106</t>
+  </si>
+  <si>
+    <t>kind%=010bj0107</t>
+  </si>
+  <si>
+    <t>kind%=0010</t>
+  </si>
+  <si>
+    <t>kind%=0133</t>
+  </si>
+  <si>
+    <t>kind%=0134</t>
+  </si>
+  <si>
+    <t>kind%=0136</t>
+  </si>
+  <si>
+    <t>kind%=0137</t>
+  </si>
+  <si>
+    <t>kind%=02ff</t>
+  </si>
+  <si>
+    <t>kind%=0121</t>
+  </si>
+  <si>
+    <t>kind%=0123</t>
+  </si>
+  <si>
+    <t>kind%=0122</t>
+  </si>
+  <si>
+    <t>kind%=0125</t>
+  </si>
+  <si>
+    <t>kind%=0141</t>
+  </si>
+  <si>
+    <t>kind%=0142</t>
+  </si>
+  <si>
+    <t>kind%=0143</t>
+  </si>
+  <si>
+    <t>kind%=0145</t>
+  </si>
+  <si>
+    <t>kind%=0146</t>
+  </si>
+  <si>
+    <t>kind%=0147</t>
+  </si>
+  <si>
+    <t>kind%=0148</t>
+  </si>
+  <si>
+    <t>kind%=0149</t>
+  </si>
+  <si>
+    <t>kind%=014a</t>
+  </si>
+  <si>
+    <t>kind%=014b</t>
+  </si>
+  <si>
+    <t>kind%=01ff</t>
+  </si>
+  <si>
+    <t>kind%=04ff</t>
+  </si>
+  <si>
+    <t>kind%=0161</t>
+  </si>
+  <si>
+    <t>kind%=0162</t>
+  </si>
+  <si>
+    <t>kind%=0163</t>
+  </si>
+  <si>
+    <t>kind%=0164</t>
+  </si>
+  <si>
+    <t>kind%=06ff</t>
+  </si>
+  <si>
+    <t>kind%=0165</t>
+  </si>
+  <si>
+    <t>kind%=0166</t>
+  </si>
+  <si>
+    <t>kind%=0167</t>
+  </si>
+  <si>
+    <t>kind%=0171</t>
+  </si>
+  <si>
+    <t>kind%=0172</t>
+  </si>
+  <si>
+    <t>kind%=0173</t>
+  </si>
+  <si>
+    <t>kind%=0174</t>
+  </si>
+  <si>
+    <t>kind%=0175</t>
+  </si>
+  <si>
+    <t>kind%=0176</t>
+  </si>
+  <si>
+    <t>kind%=0177</t>
+  </si>
+  <si>
+    <t>kind%=0178</t>
+  </si>
+  <si>
+    <t>kind%=0179</t>
+  </si>
+  <si>
+    <t>kind%=017a</t>
+  </si>
+  <si>
+    <t>kind%=84ff</t>
   </si>
 </sst>
 </file>
@@ -646,12 +646,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -681,7 +687,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -696,6 +702,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -983,8 +995,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C58"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -995,18 +1007,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="6"/>
-      <c r="C2" s="6"/>
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
@@ -1021,7 +1033,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>19</v>
@@ -1032,7 +1044,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>21</v>
@@ -1043,7 +1055,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>23</v>
@@ -1054,7 +1066,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>25</v>
@@ -1065,7 +1077,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>27</v>
@@ -1076,7 +1088,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>29</v>
@@ -1087,7 +1099,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>5</v>
@@ -1098,7 +1110,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>7</v>
@@ -1109,7 +1121,7 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>9</v>
@@ -1120,7 +1132,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>11</v>
@@ -1131,7 +1143,7 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>13</v>
@@ -1142,7 +1154,7 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>14</v>
@@ -1153,7 +1165,7 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>16</v>
@@ -1163,52 +1175,52 @@
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A17" s="4" t="s">
-        <v>121</v>
-      </c>
-      <c r="B17" s="4" t="s">
+      <c r="A17" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="B19" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="C17" s="4" t="s">
+      <c r="C19" s="7" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A18" s="4" t="s">
-        <v>122</v>
-      </c>
-      <c r="B18" s="4" t="s">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="B20" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="C18" s="4" t="s">
+      <c r="C20" s="7" t="s">
         <v>34</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A19" s="3" t="s">
-        <v>123</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A20" s="3" t="s">
-        <v>124</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="5" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="B21" s="5" t="s">
         <v>39</v>
@@ -1219,7 +1231,7 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>41</v>
@@ -1230,7 +1242,7 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B23" s="3" t="s">
         <v>43</v>
@@ -1241,7 +1253,7 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B24" s="3" t="s">
         <v>45</v>
@@ -1252,7 +1264,7 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B25" s="3" t="s">
         <v>41</v>
@@ -1262,47 +1274,47 @@
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A26" s="5" t="s">
-        <v>130</v>
-      </c>
-      <c r="B26" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="C26" s="5" t="s">
-        <v>49</v>
+      <c r="A26" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="B26" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="C26" s="6" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A27" s="5" t="s">
-        <v>131</v>
-      </c>
-      <c r="B27" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="C27" s="5" t="s">
-        <v>51</v>
+      <c r="A27" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="B27" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="C27" s="6" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" s="5" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A29" s="5" t="s">
-        <v>133</v>
-      </c>
-      <c r="B29" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="C29" s="5" t="s">
-        <v>55</v>
+      <c r="A29" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="B29" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="C29" s="6" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
@@ -1310,10 +1322,10 @@
         <v>134</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
@@ -1321,10 +1333,10 @@
         <v>135</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
@@ -1332,10 +1344,10 @@
         <v>136</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
@@ -1343,10 +1355,10 @@
         <v>137</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
@@ -1615,7 +1627,7 @@
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A58" s="4" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B58" s="4" t="s">
         <v>5</v>

</xml_diff>

<commit_message>
Fix some bug and update script
</commit_message>
<xml_diff>
--- a/conf/excel/C_BackLine.xlsx
+++ b/conf/excel/C_BackLine.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\长期文件\学习资料\综合学习资料\tencent\配置文件相关\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\76780\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20972D1D-449C-41AF-B672-1F2F3F980B64}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D915379-EC42-471D-BA1C-368602351FE2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -441,166 +441,166 @@
     <t>体育场范围线</t>
   </si>
   <si>
-    <t>kind=0242</t>
-  </si>
-  <si>
-    <t>kind=0243</t>
-  </si>
-  <si>
-    <t>kind=0244</t>
-  </si>
-  <si>
-    <t>kind=0241</t>
-  </si>
-  <si>
-    <t>kind=0245</t>
-  </si>
-  <si>
-    <t>kind=0246</t>
-  </si>
-  <si>
-    <t>kind=07ff</t>
-  </si>
-  <si>
-    <t>kind=010bj0103</t>
-  </si>
-  <si>
-    <t>kind=010bj0104</t>
-  </si>
-  <si>
-    <t>kind=010bj0109</t>
-  </si>
-  <si>
-    <t>kind=010bj0106</t>
-  </si>
-  <si>
-    <t>kind=010bj0107</t>
-  </si>
-  <si>
-    <t>kind=0010</t>
-  </si>
-  <si>
-    <t>kind=0133</t>
-  </si>
-  <si>
-    <t>kind=0134</t>
-  </si>
-  <si>
-    <t>kind=0136</t>
-  </si>
-  <si>
-    <t>kind=0137</t>
-  </si>
-  <si>
-    <t>kind=02ff</t>
-  </si>
-  <si>
-    <t>kind=0121</t>
-  </si>
-  <si>
-    <t>kind=0123</t>
-  </si>
-  <si>
-    <t>kind=0122</t>
-  </si>
-  <si>
-    <t>kind=0125</t>
-  </si>
-  <si>
-    <t>kind=0141</t>
-  </si>
-  <si>
-    <t>kind=0142</t>
-  </si>
-  <si>
-    <t>kind=0143</t>
-  </si>
-  <si>
-    <t>kind=0144</t>
-  </si>
-  <si>
-    <t>kind=0145</t>
-  </si>
-  <si>
-    <t>kind=0146</t>
-  </si>
-  <si>
-    <t>kind=0147</t>
-  </si>
-  <si>
-    <t>kind=0148</t>
-  </si>
-  <si>
-    <t>kind=0149</t>
-  </si>
-  <si>
-    <t>kind=014a</t>
-  </si>
-  <si>
-    <t>kind=014b</t>
-  </si>
-  <si>
-    <t>kind=01ff</t>
-  </si>
-  <si>
-    <t>kind=04ff</t>
-  </si>
-  <si>
-    <t>kind=0161</t>
-  </si>
-  <si>
-    <t>kind=0162</t>
-  </si>
-  <si>
-    <t>kind=0163</t>
-  </si>
-  <si>
-    <t>kind=0164</t>
-  </si>
-  <si>
-    <t>kind=06ff</t>
-  </si>
-  <si>
-    <t>kind=0165</t>
-  </si>
-  <si>
-    <t>kind=0166</t>
-  </si>
-  <si>
-    <t>kind=0167</t>
-  </si>
-  <si>
-    <t>kind=0171</t>
-  </si>
-  <si>
-    <t>kind=0172</t>
-  </si>
-  <si>
-    <t>kind=0173</t>
-  </si>
-  <si>
-    <t>kind=0174</t>
-  </si>
-  <si>
-    <t>kind=0175</t>
-  </si>
-  <si>
-    <t>kind=0176</t>
-  </si>
-  <si>
-    <t>kind=0177</t>
-  </si>
-  <si>
-    <t>kind=0178</t>
-  </si>
-  <si>
-    <t>kind=0179</t>
-  </si>
-  <si>
-    <t>kind=017a</t>
-  </si>
-  <si>
-    <t>kind=84ff</t>
+    <t>kind%=0242</t>
+  </si>
+  <si>
+    <t>kind%=0243</t>
+  </si>
+  <si>
+    <t>kind%=0244</t>
+  </si>
+  <si>
+    <t>kind%=0241</t>
+  </si>
+  <si>
+    <t>kind%=0245</t>
+  </si>
+  <si>
+    <t>kind%=0246</t>
+  </si>
+  <si>
+    <t>kind%=07ff</t>
+  </si>
+  <si>
+    <t>kind%=010bj0103</t>
+  </si>
+  <si>
+    <t>kind%=010bj0104</t>
+  </si>
+  <si>
+    <t>kind%=010bj0109</t>
+  </si>
+  <si>
+    <t>kind%=010bj0106</t>
+  </si>
+  <si>
+    <t>kind%=010bj0107</t>
+  </si>
+  <si>
+    <t>kind%=0010</t>
+  </si>
+  <si>
+    <t>kind%=0133</t>
+  </si>
+  <si>
+    <t>kind%=0134</t>
+  </si>
+  <si>
+    <t>kind%=0136</t>
+  </si>
+  <si>
+    <t>kind%=0137</t>
+  </si>
+  <si>
+    <t>kind%=02ff</t>
+  </si>
+  <si>
+    <t>kind%=0121</t>
+  </si>
+  <si>
+    <t>kind%=0123</t>
+  </si>
+  <si>
+    <t>kind%=0122</t>
+  </si>
+  <si>
+    <t>kind%=0125</t>
+  </si>
+  <si>
+    <t>kind%=0141</t>
+  </si>
+  <si>
+    <t>kind%=0142</t>
+  </si>
+  <si>
+    <t>kind%=0143</t>
+  </si>
+  <si>
+    <t>kind%=0144</t>
+  </si>
+  <si>
+    <t>kind%=0145</t>
+  </si>
+  <si>
+    <t>kind%=0146</t>
+  </si>
+  <si>
+    <t>kind%=0147</t>
+  </si>
+  <si>
+    <t>kind%=0148</t>
+  </si>
+  <si>
+    <t>kind%=0149</t>
+  </si>
+  <si>
+    <t>kind%=014a</t>
+  </si>
+  <si>
+    <t>kind%=014b</t>
+  </si>
+  <si>
+    <t>kind%=01ff</t>
+  </si>
+  <si>
+    <t>kind%=04ff</t>
+  </si>
+  <si>
+    <t>kind%=0161</t>
+  </si>
+  <si>
+    <t>kind%=0162</t>
+  </si>
+  <si>
+    <t>kind%=0163</t>
+  </si>
+  <si>
+    <t>kind%=0164</t>
+  </si>
+  <si>
+    <t>kind%=06ff</t>
+  </si>
+  <si>
+    <t>kind%=0165</t>
+  </si>
+  <si>
+    <t>kind%=0166</t>
+  </si>
+  <si>
+    <t>kind%=0167</t>
+  </si>
+  <si>
+    <t>kind%=0171</t>
+  </si>
+  <si>
+    <t>kind%=0172</t>
+  </si>
+  <si>
+    <t>kind%=0173</t>
+  </si>
+  <si>
+    <t>kind%=0174</t>
+  </si>
+  <si>
+    <t>kind%=0175</t>
+  </si>
+  <si>
+    <t>kind%=0176</t>
+  </si>
+  <si>
+    <t>kind%=0177</t>
+  </si>
+  <si>
+    <t>kind%=0178</t>
+  </si>
+  <si>
+    <t>kind%=0179</t>
+  </si>
+  <si>
+    <t>kind%=017a</t>
+  </si>
+  <si>
+    <t>kind%=84ff</t>
   </si>
 </sst>
 </file>

</xml_diff>